<commit_message>
updated results tracker property names; also added sub properties of the resource tracker property assoc.file.result.depends.on; sub properties are result.id and result.id.depends.on; result.id is replaced by resultID and result.id.depends.on is replaced by resultIdDependsOn
</commit_message>
<xml_diff>
--- a/schema-dot-names.xlsx
+++ b/schema-dot-names.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tentner-andrea\project_repositories\dsc\heal-data-pkg-tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC379C8-A427-4792-B39B-3A9E9B7E6B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F62ADA-C815-4D59-AFF1-25650C464E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{5AF35D0D-5205-4BF7-A780-2F19026420A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5AF35D0D-5205-4BF7-A780-2F19026420A7}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment-tracker" sheetId="1" r:id="rId1"/>
-    <sheet name="resource-tracker" sheetId="2" r:id="rId2"/>
-    <sheet name="results-tracker" sheetId="3" r:id="rId3"/>
+    <sheet name="results-tracker" sheetId="3" r:id="rId2"/>
+    <sheet name="resource-tracker" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="87">
   <si>
     <t>resource-tracker</t>
   </si>
@@ -187,6 +187,9 @@
     <t>change-to</t>
   </si>
   <si>
+    <t>resource.id.num</t>
+  </si>
+  <si>
     <t>categorySubData</t>
   </si>
   <si>
@@ -284,6 +287,18 @@
   </si>
   <si>
     <t>annotationModTimeStamp</t>
+  </si>
+  <si>
+    <t>result.id.depends.on</t>
+  </si>
+  <si>
+    <t>resultIdDependsOn</t>
+  </si>
+  <si>
+    <t>resource-tracker:assoc.file.result.depends.on</t>
+  </si>
+  <si>
+    <t>resourceIdNumber</t>
   </si>
 </sst>
 </file>
@@ -704,7 +719,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -715,7 +730,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -737,7 +752,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -748,7 +763,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -757,381 +772,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E796FFCD-2282-41C8-86A3-5449625A1B92}">
-  <dimension ref="A1:C32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="35.88671875" customWidth="1"/>
-    <col min="3" max="3" width="37.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B32">
-    <sortCondition ref="B2:B32"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{536B3DEC-77BA-4E4B-9034-8DFB006AACD9}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -1165,7 +805,7 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1176,7 +816,7 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1209,7 +849,7 @@
         <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1220,7 +860,7 @@
         <v>36</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1231,7 +871,7 @@
         <v>37</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1242,10 +882,10 @@
         <v>46</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1256,7 +896,7 @@
         <v>40</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1267,10 +907,10 @@
         <v>45</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1281,7 +921,7 @@
         <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1292,7 +932,7 @@
         <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1301,4 +941,409 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E796FFCD-2282-41C8-86A3-5449625A1B92}">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="41.109375" customWidth="1"/>
+    <col min="2" max="2" width="35.88671875" customWidth="1"/>
+    <col min="3" max="3" width="37.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B32">
+    <sortCondition ref="B2:B32"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
udpated property names for resource tracker
</commit_message>
<xml_diff>
--- a/schema-dot-names.xlsx
+++ b/schema-dot-names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tentner-andrea\project_repositories\dsc\heal-data-pkg-tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F62ADA-C815-4D59-AFF1-25650C464E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5315B8EF-3EF0-46B0-984A-9696032F2BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5AF35D0D-5205-4BF7-A780-2F19026420A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{5AF35D0D-5205-4BF7-A780-2F19026420A7}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment-tracker" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="86">
   <si>
     <t>resource-tracker</t>
   </si>
@@ -200,9 +200,6 @@
   </si>
   <si>
     <t>expBelongsTo</t>
-  </si>
-  <si>
-    <t>accessType</t>
   </si>
   <si>
     <t>accessDate</t>
@@ -719,7 +716,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -730,7 +727,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -752,7 +749,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -763,7 +760,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -775,7 +772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{536B3DEC-77BA-4E4B-9034-8DFB006AACD9}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -805,7 +802,7 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -816,7 +813,7 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -849,7 +846,7 @@
         <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -860,7 +857,7 @@
         <v>36</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -871,7 +868,7 @@
         <v>37</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -882,10 +879,10 @@
         <v>46</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -896,7 +893,7 @@
         <v>40</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -907,10 +904,10 @@
         <v>45</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -921,7 +918,7 @@
         <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -932,7 +929,7 @@
         <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -947,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E796FFCD-2282-41C8-86A3-5449625A1B92}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -977,7 +974,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -988,7 +985,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -999,7 +996,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1010,7 +1007,7 @@
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1021,7 +1018,7 @@
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1032,7 +1029,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1043,7 +1040,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1054,7 +1051,7 @@
         <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1120,7 +1117,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1131,7 +1128,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1142,7 +1139,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1186,7 +1183,7 @@
         <v>29</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1241,7 +1238,7 @@
         <v>34</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1252,7 +1249,7 @@
         <v>11</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1263,7 +1260,7 @@
         <v>35</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1274,7 +1271,7 @@
         <v>36</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1285,7 +1282,7 @@
         <v>37</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1312,24 +1309,24 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B33" t="s">
         <v>40</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1337,7 +1334,7 @@
         <v>49</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>